<commit_message>
Updating spreads on 19-Jun-24
</commit_message>
<xml_diff>
--- a/spreads/intc.xlsx
+++ b/spreads/intc.xlsx
@@ -441,7 +441,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>+$0.61 (+1.77%)</t>
+          <t>-$0.32 (-1.01%)</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
         <v>54228</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>54228</v>
+        <v>55237</v>
       </c>
     </row>
     <row r="4">
@@ -610,7 +610,7 @@
         <v>54228</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>54228</v>
+        <v>55237</v>
       </c>
     </row>
     <row r="5">
@@ -688,7 +688,7 @@
         <v>-32517</v>
       </c>
       <c r="M6" s="1" t="n">
-        <v>-32517</v>
+        <v>-32317</v>
       </c>
     </row>
     <row r="7">
@@ -729,7 +729,7 @@
         <v>21711</v>
       </c>
       <c r="M7" s="1" t="n">
-        <v>21711</v>
+        <v>22920</v>
       </c>
     </row>
     <row r="8">
@@ -807,7 +807,7 @@
         <v>0.4</v>
       </c>
       <c r="M9" s="3" t="n">
-        <v>0.4</v>
+        <v>0.415</v>
       </c>
     </row>
     <row r="10">
@@ -848,7 +848,7 @@
         <v>-5634</v>
       </c>
       <c r="M10" s="1" t="n">
-        <v>-5634</v>
+        <v>-5887</v>
       </c>
     </row>
     <row r="11">
@@ -889,7 +889,7 @@
         <v>-16046</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>-16046</v>
+        <v>-16319</v>
       </c>
     </row>
     <row r="12">
@@ -976,7 +976,7 @@
         <v>-21680</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>-21680</v>
+        <v>-22206</v>
       </c>
     </row>
     <row r="15">
@@ -1017,7 +1017,7 @@
         <v>31</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>31</v>
+        <v>714</v>
       </c>
     </row>
     <row r="16">
@@ -1095,7 +1095,7 @@
         <v>0.001</v>
       </c>
       <c r="M17" s="3" t="n">
-        <v>0.001</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="18">
@@ -1136,7 +1136,7 @@
         <v>-878</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>-878</v>
+        <v>-943</v>
       </c>
     </row>
     <row r="19">
@@ -1177,7 +1177,7 @@
         <v>1335</v>
       </c>
       <c r="M19" s="1" t="n">
-        <v>1335</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="20">
@@ -1237,7 +1237,7 @@
         <v>106</v>
       </c>
       <c r="M21" s="2" t="n">
-        <v>106</v>
+        <v>451</v>
       </c>
     </row>
     <row r="22">
@@ -1278,7 +1278,7 @@
         <v>66</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>66</v>
+        <v>-199</v>
       </c>
     </row>
     <row r="23">
@@ -1318,8 +1318,8 @@
       <c r="L23" s="2" t="n">
         <v>660</v>
       </c>
-      <c r="M23" s="2" t="n">
-        <v>660</v>
+      <c r="M23" s="1" t="n">
+        <v>1347</v>
       </c>
     </row>
     <row r="24">
@@ -1360,7 +1360,7 @@
         <v>-222</v>
       </c>
       <c r="M24" s="2" t="n">
-        <v>-222</v>
+        <v>-390</v>
       </c>
     </row>
     <row r="25">
@@ -1380,7 +1380,9 @@
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
+      <c r="M25" s="2" t="n">
+        <v>-222</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1420,7 +1422,7 @@
         <v>40</v>
       </c>
       <c r="M26" s="2" t="n">
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27">
@@ -1476,7 +1478,7 @@
         <v>-45</v>
       </c>
       <c r="M28" s="2" t="n">
-        <v>-45</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="29">
@@ -1545,7 +1547,7 @@
         <v>329</v>
       </c>
       <c r="M31" s="2" t="n">
-        <v>329</v>
+        <v>406</v>
       </c>
     </row>
     <row r="32">
@@ -1608,8 +1610,8 @@
       <c r="L33" s="2" t="n">
         <v>762</v>
       </c>
-      <c r="M33" s="2" t="n">
-        <v>762</v>
+      <c r="M33" s="1" t="n">
+        <v>1201</v>
       </c>
     </row>
     <row r="34">
@@ -1649,8 +1651,8 @@
       <c r="L34" s="2" t="n">
         <v>913</v>
       </c>
-      <c r="M34" s="2" t="n">
-        <v>913</v>
+      <c r="M34" s="1" t="n">
+        <v>2805</v>
       </c>
     </row>
     <row r="35">
@@ -1691,7 +1693,7 @@
         <v>1675</v>
       </c>
       <c r="M35" s="1" t="n">
-        <v>1675</v>
+        <v>4006</v>
       </c>
     </row>
     <row r="36">
@@ -1732,7 +1734,7 @@
         <v>1675</v>
       </c>
       <c r="M36" s="1" t="n">
-        <v>1675</v>
+        <v>4006</v>
       </c>
     </row>
     <row r="37">
@@ -1757,7 +1759,7 @@
         <v>14</v>
       </c>
       <c r="M37" s="2" t="n">
-        <v>14</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38">
@@ -1798,7 +1800,7 @@
         <v>1689</v>
       </c>
       <c r="M38" s="1" t="n">
-        <v>1689</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="39">
@@ -1839,7 +1841,7 @@
         <v>1689</v>
       </c>
       <c r="M39" s="1" t="n">
-        <v>1689</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="40">
@@ -1880,7 +1882,7 @@
         <v>0.031</v>
       </c>
       <c r="M40" s="3" t="n">
-        <v>0.031</v>
+        <v>0.07400000000000001</v>
       </c>
     </row>
     <row r="41">
@@ -1921,7 +1923,7 @@
         <v>1689</v>
       </c>
       <c r="M41" s="1" t="n">
-        <v>1689</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="42">
@@ -1962,7 +1964,7 @@
         <v>0.031</v>
       </c>
       <c r="M42" s="3" t="n">
-        <v>0.031</v>
+        <v>0.07400000000000001</v>
       </c>
     </row>
     <row r="43">
@@ -2010,7 +2012,7 @@
         <v>0.4</v>
       </c>
       <c r="M44" s="2" t="n">
-        <v>0.4</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="45">
@@ -2088,7 +2090,7 @@
         <v>4212</v>
       </c>
       <c r="M46" s="1" t="n">
-        <v>4212</v>
+        <v>4234</v>
       </c>
     </row>
     <row r="47">
@@ -2166,7 +2168,7 @@
         <v>4190</v>
       </c>
       <c r="M48" s="1" t="n">
-        <v>4190</v>
+        <v>4212</v>
       </c>
     </row>
     <row r="49">
@@ -2244,7 +2246,7 @@
         <v>0.74</v>
       </c>
       <c r="M50" s="2" t="n">
-        <v>0.74</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="51">
@@ -2322,7 +2324,7 @@
         <v>1.828</v>
       </c>
       <c r="M52" s="3" t="n">
-        <v>1.828</v>
+        <v>0.518</v>
       </c>
     </row>
     <row r="53">
@@ -2363,7 +2365,7 @@
         <v>0.4</v>
       </c>
       <c r="M53" s="2" t="n">
-        <v>0.4</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="54">
@@ -2404,7 +2406,7 @@
         <v>9633</v>
       </c>
       <c r="M54" s="1" t="n">
-        <v>9633</v>
+        <v>10501</v>
       </c>
     </row>
     <row r="55">
@@ -2481,9 +2483,7 @@
       <c r="L56" s="1" t="n">
         <v>10040</v>
       </c>
-      <c r="M56" s="1" t="n">
-        <v>10040</v>
-      </c>
+      <c r="M56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2523,7 +2523,7 @@
         <v>17281</v>
       </c>
       <c r="M57" s="1" t="n">
-        <v>17281</v>
+        <v>17554</v>
       </c>
     </row>
     <row r="58">
@@ -2605,7 +2605,7 @@
         <v>-119.8</v>
       </c>
       <c r="M59" s="2" t="n">
-        <v>-119.8</v>
+        <v>-233.6</v>
       </c>
     </row>
   </sheetData>
@@ -2732,7 +2732,7 @@
         <v>7079</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>7079</v>
+        <v>6923</v>
       </c>
     </row>
     <row r="4">
@@ -2773,7 +2773,7 @@
         <v>17955</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>17955</v>
+        <v>14388</v>
       </c>
     </row>
     <row r="5">
@@ -2847,7 +2847,7 @@
         <v>25034</v>
       </c>
       <c r="M6" s="1" t="n">
-        <v>25034</v>
+        <v>21311</v>
       </c>
     </row>
     <row r="7">
@@ -2888,7 +2888,7 @@
         <v>3402</v>
       </c>
       <c r="M7" s="1" t="n">
-        <v>3402</v>
+        <v>3323</v>
       </c>
     </row>
     <row r="8">
@@ -2928,8 +2928,8 @@
       <c r="L8" s="2" t="n">
         <v>204</v>
       </c>
-      <c r="M8" s="2" t="n">
-        <v>204</v>
+      <c r="M8" s="1" t="n">
+        <v>2150</v>
       </c>
     </row>
     <row r="9">
@@ -3005,7 +3005,7 @@
         <v>3606</v>
       </c>
       <c r="M10" s="1" t="n">
-        <v>3606</v>
+        <v>5473</v>
       </c>
     </row>
     <row r="11">
@@ -3046,7 +3046,7 @@
         <v>11127</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>11127</v>
+        <v>11494</v>
       </c>
     </row>
     <row r="12">
@@ -3108,7 +3108,7 @@
         <v>3502</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>3502</v>
+        <v>4330</v>
       </c>
     </row>
     <row r="14">
@@ -3149,7 +3149,7 @@
         <v>43269</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>43269</v>
+        <v>42608</v>
       </c>
     </row>
     <row r="15">
@@ -3190,7 +3190,7 @@
         <v>195162</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>195162</v>
+        <v>199239</v>
       </c>
     </row>
     <row r="16">
@@ -3231,7 +3231,7 @@
         <v>-98010</v>
       </c>
       <c r="M16" s="1" t="n">
-        <v>-98010</v>
+        <v>-99315</v>
       </c>
     </row>
     <row r="17">
@@ -3272,7 +3272,7 @@
         <v>97152</v>
       </c>
       <c r="M17" s="1" t="n">
-        <v>97152</v>
+        <v>99924</v>
       </c>
     </row>
     <row r="18">
@@ -3313,7 +3313,7 @@
         <v>5829</v>
       </c>
       <c r="M18" s="1" t="n">
-        <v>5829</v>
+        <v>6139</v>
       </c>
     </row>
     <row r="19">
@@ -3354,7 +3354,7 @@
         <v>27591</v>
       </c>
       <c r="M19" s="1" t="n">
-        <v>27591</v>
+        <v>27440</v>
       </c>
     </row>
     <row r="20">
@@ -3395,7 +3395,7 @@
         <v>4589</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>4589</v>
+        <v>4675</v>
       </c>
     </row>
     <row r="21">
@@ -3470,9 +3470,7 @@
       <c r="L22" s="1" t="n">
         <v>5459</v>
       </c>
-      <c r="M22" s="1" t="n">
-        <v>5459</v>
-      </c>
+      <c r="M22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3512,7 +3510,7 @@
         <v>7683</v>
       </c>
       <c r="M23" s="1" t="n">
-        <v>7683</v>
+        <v>11947</v>
       </c>
     </row>
     <row r="24">
@@ -3553,7 +3551,7 @@
         <v>191572</v>
       </c>
       <c r="M24" s="1" t="n">
-        <v>191572</v>
+        <v>192733</v>
       </c>
     </row>
     <row r="25">
@@ -3594,7 +3592,7 @@
         <v>8578</v>
       </c>
       <c r="M25" s="1" t="n">
-        <v>8578</v>
+        <v>8559</v>
       </c>
     </row>
     <row r="26">
@@ -3635,7 +3633,7 @@
         <v>14818</v>
       </c>
       <c r="M26" s="1" t="n">
-        <v>14818</v>
+        <v>13234</v>
       </c>
     </row>
     <row r="27">
@@ -3667,7 +3665,9 @@
         <v>3944</v>
       </c>
       <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
+      <c r="M27" s="2" t="n">
+        <v>793</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3707,7 +3707,7 @@
         <v>2324</v>
       </c>
       <c r="M28" s="1" t="n">
-        <v>2324</v>
+        <v>3788</v>
       </c>
     </row>
     <row r="29">
@@ -3729,9 +3729,7 @@
       <c r="L29" s="2" t="n">
         <v>622</v>
       </c>
-      <c r="M29" s="2" t="n">
-        <v>622</v>
-      </c>
+      <c r="M29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3770,8 +3768,8 @@
       <c r="L30" s="1" t="n">
         <v>1107</v>
       </c>
-      <c r="M30" s="1" t="n">
-        <v>1107</v>
+      <c r="M30" s="2" t="n">
+        <v>346</v>
       </c>
     </row>
     <row r="31">
@@ -3862,7 +3860,7 @@
         <v>604</v>
       </c>
       <c r="M33" s="2" t="n">
-        <v>604</v>
+        <v>493</v>
       </c>
     </row>
     <row r="34">
@@ -3903,7 +3901,7 @@
         <v>28053</v>
       </c>
       <c r="M34" s="1" t="n">
-        <v>28053</v>
+        <v>27213</v>
       </c>
     </row>
     <row r="35">
@@ -3944,7 +3942,7 @@
         <v>46978</v>
       </c>
       <c r="M35" s="1" t="n">
-        <v>46978</v>
+        <v>47869</v>
       </c>
     </row>
     <row r="36">
@@ -3966,9 +3964,7 @@
       <c r="L36" s="2" t="n">
         <v>359</v>
       </c>
-      <c r="M36" s="2" t="n">
-        <v>359</v>
-      </c>
+      <c r="M36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4036,9 +4032,7 @@
       <c r="L38" s="2" t="n">
         <v>675</v>
       </c>
-      <c r="M38" s="2" t="n">
-        <v>675</v>
-      </c>
+      <c r="M38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4077,9 +4071,7 @@
       <c r="L39" s="2" t="n">
         <v>186</v>
       </c>
-      <c r="M39" s="2" t="n">
-        <v>186</v>
-      </c>
+      <c r="M39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4119,7 +4111,7 @@
         <v>5356</v>
       </c>
       <c r="M40" s="1" t="n">
-        <v>5356</v>
+        <v>6895</v>
       </c>
     </row>
     <row r="41">
@@ -4160,7 +4152,7 @@
         <v>81607</v>
       </c>
       <c r="M41" s="1" t="n">
-        <v>81607</v>
+        <v>81977</v>
       </c>
     </row>
     <row r="42">
@@ -4201,7 +4193,7 @@
         <v>36649</v>
       </c>
       <c r="M42" s="1" t="n">
-        <v>36649</v>
+        <v>38291</v>
       </c>
     </row>
     <row r="43">
@@ -4242,7 +4234,7 @@
         <v>69156</v>
       </c>
       <c r="M43" s="1" t="n">
-        <v>69156</v>
+        <v>68224</v>
       </c>
     </row>
     <row r="44">
@@ -4283,7 +4275,7 @@
         <v>-215</v>
       </c>
       <c r="M44" s="2" t="n">
-        <v>-215</v>
+        <v>-542</v>
       </c>
     </row>
     <row r="45">
@@ -4324,7 +4316,7 @@
         <v>105590</v>
       </c>
       <c r="M45" s="1" t="n">
-        <v>105590</v>
+        <v>105973</v>
       </c>
     </row>
     <row r="46">
@@ -4349,7 +4341,7 @@
         <v>4375</v>
       </c>
       <c r="M46" s="1" t="n">
-        <v>4375</v>
+        <v>4783</v>
       </c>
     </row>
     <row r="47">
@@ -4390,7 +4382,7 @@
         <v>109965</v>
       </c>
       <c r="M47" s="1" t="n">
-        <v>109965</v>
+        <v>110756</v>
       </c>
     </row>
     <row r="48">
@@ -4431,7 +4423,7 @@
         <v>191572</v>
       </c>
       <c r="M48" s="1" t="n">
-        <v>191572</v>
+        <v>192733</v>
       </c>
     </row>
     <row r="49">
@@ -4479,7 +4471,7 @@
         <v>4228</v>
       </c>
       <c r="M50" s="1" t="n">
-        <v>4228</v>
+        <v>4257</v>
       </c>
     </row>
     <row r="51">
@@ -4520,7 +4512,7 @@
         <v>24.97</v>
       </c>
       <c r="M51" s="2" t="n">
-        <v>24.97</v>
+        <v>24.89</v>
       </c>
     </row>
     <row r="52">
@@ -4561,7 +4553,7 @@
         <v>73410</v>
       </c>
       <c r="M52" s="1" t="n">
-        <v>73410</v>
+        <v>73858</v>
       </c>
     </row>
     <row r="53">
@@ -4602,7 +4594,7 @@
         <v>17.36</v>
       </c>
       <c r="M53" s="2" t="n">
-        <v>17.36</v>
+        <v>17.35</v>
       </c>
     </row>
     <row r="54">
@@ -4643,7 +4635,7 @@
         <v>50283</v>
       </c>
       <c r="M54" s="1" t="n">
-        <v>50283</v>
+        <v>52450</v>
       </c>
     </row>
     <row r="55">
@@ -4684,7 +4676,7 @@
         <v>24055</v>
       </c>
       <c r="M55" s="1" t="n">
-        <v>24055</v>
+        <v>29668</v>
       </c>
     </row>
     <row r="56">
@@ -4906,7 +4898,7 @@
         <v>1689</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>1689</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="4">
@@ -4947,7 +4939,7 @@
         <v>7847</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>7847</v>
+        <v>8146</v>
       </c>
     </row>
     <row r="5">
@@ -4988,7 +4980,7 @@
         <v>1755</v>
       </c>
       <c r="M5" s="1" t="n">
-        <v>1755</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="6">
@@ -5029,7 +5021,7 @@
         <v>9602</v>
       </c>
       <c r="M6" s="1" t="n">
-        <v>9602</v>
+        <v>9787</v>
       </c>
     </row>
     <row r="7">
@@ -5131,7 +5123,7 @@
         <v>-95</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>-95</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11">
@@ -5172,7 +5164,7 @@
         <v>-42</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>-42</v>
+        <v>-83</v>
       </c>
     </row>
     <row r="12">
@@ -5213,7 +5205,7 @@
         <v>3229</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>3229</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="13">
@@ -5269,7 +5261,7 @@
         <v>-343</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>-343</v>
+        <v>-389</v>
       </c>
     </row>
     <row r="15">
@@ -5329,7 +5321,7 @@
         <v>731</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>731</v>
+        <v>525</v>
       </c>
     </row>
     <row r="17">
@@ -5370,7 +5362,7 @@
         <v>2097</v>
       </c>
       <c r="M17" s="1" t="n">
-        <v>2097</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="18">
@@ -5411,7 +5403,7 @@
         <v>-801</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>-801</v>
+        <v>-416</v>
       </c>
     </row>
     <row r="19">
@@ -5483,7 +5475,7 @@
         <v>-3531</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>-3531</v>
+        <v>-5466</v>
       </c>
     </row>
     <row r="21">
@@ -5524,7 +5516,7 @@
         <v>-1065</v>
       </c>
       <c r="M21" s="1" t="n">
-        <v>-1065</v>
+        <v>-1358</v>
       </c>
     </row>
     <row r="22">
@@ -5565,7 +5557,7 @@
         <v>11471</v>
       </c>
       <c r="M22" s="1" t="n">
-        <v>11471</v>
+        <v>12033</v>
       </c>
     </row>
     <row r="23">
@@ -5606,7 +5598,7 @@
         <v>-2569</v>
       </c>
       <c r="M23" s="1" t="n">
-        <v>-2569</v>
+        <v>-5215</v>
       </c>
     </row>
     <row r="24">
@@ -5647,7 +5639,7 @@
         <v>-25750</v>
       </c>
       <c r="M24" s="1" t="n">
-        <v>-25750</v>
+        <v>-24307</v>
       </c>
     </row>
     <row r="25">
@@ -5764,8 +5756,8 @@
       <c r="L28" s="2" t="n">
         <v>-264</v>
       </c>
-      <c r="M28" s="2" t="n">
-        <v>-264</v>
+      <c r="M28" s="1" t="n">
+        <v>4833</v>
       </c>
     </row>
     <row r="29">
@@ -5827,7 +5819,7 @@
         <v>1973</v>
       </c>
       <c r="M30" s="1" t="n">
-        <v>1973</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="31">
@@ -5868,7 +5860,7 @@
         <v>-24041</v>
       </c>
       <c r="M31" s="1" t="n">
-        <v>-24041</v>
+        <v>-18083</v>
       </c>
     </row>
     <row r="32">
@@ -5909,7 +5901,7 @@
         <v>11391</v>
       </c>
       <c r="M32" s="1" t="n">
-        <v>11391</v>
+        <v>3753</v>
       </c>
     </row>
     <row r="33">
@@ -5946,7 +5938,7 @@
         <v>-4463</v>
       </c>
       <c r="M33" s="1" t="n">
-        <v>-4463</v>
+        <v>-1518</v>
       </c>
     </row>
     <row r="34">
@@ -5987,7 +5979,7 @@
         <v>1042</v>
       </c>
       <c r="M34" s="1" t="n">
-        <v>1042</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="35">
@@ -6063,7 +6055,7 @@
         <v>-3088</v>
       </c>
       <c r="M36" s="1" t="n">
-        <v>-3088</v>
+        <v>-2105</v>
       </c>
     </row>
     <row r="37">
@@ -6104,7 +6096,7 @@
         <v>-3088</v>
       </c>
       <c r="M37" s="1" t="n">
-        <v>-3088</v>
+        <v>-2105</v>
       </c>
     </row>
     <row r="38">
@@ -6145,7 +6137,7 @@
         <v>3623</v>
       </c>
       <c r="M38" s="1" t="n">
-        <v>3623</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="39">
@@ -6186,7 +6178,7 @@
         <v>8505</v>
       </c>
       <c r="M39" s="1" t="n">
-        <v>8505</v>
+        <v>4741</v>
       </c>
     </row>
     <row r="40">
@@ -6248,7 +6240,7 @@
         <v>-4065</v>
       </c>
       <c r="M41" s="1" t="n">
-        <v>-4065</v>
+        <v>-1309</v>
       </c>
     </row>
     <row r="42">
@@ -6296,7 +6288,7 @@
         <v>-14279</v>
       </c>
       <c r="M43" s="1" t="n">
-        <v>-14279</v>
+        <v>-12274</v>
       </c>
     </row>
     <row r="44">
@@ -6374,7 +6366,7 @@
         <v>-26.3</v>
       </c>
       <c r="M45" s="2" t="n">
-        <v>-26.3</v>
+        <v>-22.2</v>
       </c>
     </row>
     <row r="46">
@@ -6415,7 +6407,7 @@
         <v>11144</v>
       </c>
       <c r="M46" s="1" t="n">
-        <v>11144</v>
+        <v>7079</v>
       </c>
     </row>
     <row r="47">
@@ -6456,7 +6448,7 @@
         <v>7079</v>
       </c>
       <c r="M47" s="1" t="n">
-        <v>7079</v>
+        <v>6923</v>
       </c>
     </row>
     <row r="48">
@@ -6497,7 +6489,7 @@
         <v>613</v>
       </c>
       <c r="M48" s="2" t="n">
-        <v>613</v>
+        <v>914</v>
       </c>
     </row>
     <row r="49">
@@ -6538,7 +6530,7 @@
         <v>2621</v>
       </c>
       <c r="M49" s="1" t="n">
-        <v>2621</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="50">
@@ -6579,7 +6571,7 @@
         <v>-3.41</v>
       </c>
       <c r="M50" s="2" t="n">
-        <v>-3.41</v>
+        <v>-2.91</v>
       </c>
     </row>
   </sheetData>
@@ -6834,7 +6826,7 @@
       </c>
       <c r="AU1" t="inlineStr">
         <is>
-          <t>4/25/24</t>
+          <t>5/22/24</t>
         </is>
       </c>
     </row>
@@ -7058,7 +7050,7 @@
       </c>
       <c r="AU3" t="inlineStr">
         <is>
-          <t>2.99x</t>
+          <t>2.91x</t>
         </is>
       </c>
     </row>
@@ -7275,7 +7267,7 @@
       </c>
       <c r="AU4" t="inlineStr">
         <is>
-          <t>2.51x</t>
+          <t>2.31x</t>
         </is>
       </c>
     </row>
@@ -7492,7 +7484,7 @@
       </c>
       <c r="AU5" t="inlineStr">
         <is>
-          <t>9.67x</t>
+          <t>10.38x</t>
         </is>
       </c>
     </row>
@@ -7684,7 +7676,7 @@
       </c>
       <c r="AP6" t="inlineStr">
         <is>
-          <t>64.71x</t>
+          <t>62.09x</t>
         </is>
       </c>
       <c r="AQ6" t="inlineStr">
@@ -7709,7 +7701,7 @@
       </c>
       <c r="AU6" t="inlineStr">
         <is>
-          <t>23.04x</t>
+          <t>28.25x</t>
         </is>
       </c>
     </row>
@@ -7926,7 +7918,7 @@
       </c>
       <c r="AU7" t="inlineStr">
         <is>
-          <t>21.67x</t>
+          <t>24.90x</t>
         </is>
       </c>
     </row>
@@ -8130,7 +8122,7 @@
         <v>-34.13</v>
       </c>
       <c r="AU8" s="2" t="n">
-        <v>-25.15</v>
+        <v>-18.51</v>
       </c>
     </row>
     <row r="9">
@@ -8265,7 +8257,7 @@
         <v>-2.9</v>
       </c>
       <c r="AU9" s="2" t="n">
-        <v>-4</v>
+        <v>-5.4</v>
       </c>
     </row>
     <row r="10">
@@ -8400,7 +8392,7 @@
         <v>0.011</v>
       </c>
       <c r="AU10" s="3" t="n">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="11">
@@ -8619,7 +8611,7 @@
       </c>
       <c r="AU12" t="inlineStr">
         <is>
-          <t>3.28x</t>
+          <t>3.05x</t>
         </is>
       </c>
     </row>
@@ -8832,7 +8824,7 @@
       </c>
       <c r="AU13" t="inlineStr">
         <is>
-          <t>2.76x</t>
+          <t>2.42x</t>
         </is>
       </c>
     </row>
@@ -8903,12 +8895,12 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>7.30x</t>
+          <t>7.25x</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>7.42x</t>
+          <t>7.46x</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -8923,7 +8915,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>5.46x</t>
+          <t>5.48x</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -8938,7 +8930,7 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>6.83x</t>
+          <t>6.88x</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -8978,7 +8970,7 @@
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>8.75x</t>
+          <t>8.70x</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
@@ -8993,7 +8985,7 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>7.95x</t>
+          <t>7.88x</t>
         </is>
       </c>
       <c r="AA15" t="inlineStr">
@@ -9083,7 +9075,7 @@
       </c>
       <c r="AR15" t="inlineStr">
         <is>
-          <t>20.03x</t>
+          <t>19.82x</t>
         </is>
       </c>
       <c r="AS15" t="inlineStr">
@@ -9098,7 +9090,7 @@
       </c>
       <c r="AU15" t="inlineStr">
         <is>
-          <t>18.47x</t>
+          <t>16.02x</t>
         </is>
       </c>
     </row>
@@ -9305,7 +9297,7 @@
       </c>
       <c r="AU16" t="inlineStr">
         <is>
-          <t>5,738.35x</t>
+          <t>235.58x</t>
         </is>
       </c>
     </row>
@@ -9500,7 +9492,7 @@
         <v>-48</v>
       </c>
       <c r="AR17" s="2" t="n">
-        <v>-154.01</v>
+        <v>-154.23</v>
       </c>
       <c r="AS17" s="2" t="n">
         <v>-127.31</v>
@@ -9512,7 +9504,7 @@
       </c>
       <c r="AU17" t="inlineStr">
         <is>
-          <t>87.77x</t>
+          <t>32.89x</t>
         </is>
       </c>
     </row>
@@ -9530,12 +9522,12 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2.88x</t>
+          <t>2.86x</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>3.22x</t>
+          <t>3.25x</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -9550,129 +9542,129 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2.37x</t>
+          <t>2.38x</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
+          <t>2.90x</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>2.51x</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>2.52x</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
           <t>2.91x</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>2.51x</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>2.53x</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>2.72x</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>2.58x</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>2.38x</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>2.61x</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>3.05x</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>3.54x</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>3.30x</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>3.14x</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>2.99x</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>3.25x</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
         <is>
           <t>2.91x</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>2.72x</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>3.03x</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>3.55x</t>
+        </is>
+      </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>2.92x</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>3.19x</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>2.59x</t>
+        </is>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>2.59x</t>
+        </is>
+      </c>
+      <c r="AH18" t="inlineStr">
+        <is>
+          <t>3.25x</t>
+        </is>
+      </c>
+      <c r="AI18" t="inlineStr">
+        <is>
+          <t>2.83x</t>
+        </is>
+      </c>
+      <c r="AJ18" t="inlineStr">
         <is>
           <t>2.58x</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>2.38x</t>
-        </is>
-      </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>2.61x</t>
-        </is>
-      </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>3.05x</t>
-        </is>
-      </c>
-      <c r="V18" t="inlineStr">
-        <is>
-          <t>3.54x</t>
-        </is>
-      </c>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t>3.31x</t>
-        </is>
-      </c>
-      <c r="X18" t="inlineStr">
-        <is>
-          <t>3.14x</t>
-        </is>
-      </c>
-      <c r="Y18" t="inlineStr">
-        <is>
-          <t>2.99x</t>
-        </is>
-      </c>
-      <c r="Z18" t="inlineStr">
-        <is>
-          <t>3.28x</t>
-        </is>
-      </c>
-      <c r="AA18" t="inlineStr">
-        <is>
-          <t>2.91x</t>
-        </is>
-      </c>
-      <c r="AB18" t="inlineStr">
-        <is>
-          <t>3.03x</t>
-        </is>
-      </c>
-      <c r="AC18" t="inlineStr">
-        <is>
-          <t>3.55x</t>
-        </is>
-      </c>
-      <c r="AD18" t="inlineStr">
-        <is>
-          <t>2.90x</t>
-        </is>
-      </c>
-      <c r="AE18" t="inlineStr">
-        <is>
-          <t>3.21x</t>
-        </is>
-      </c>
-      <c r="AF18" t="inlineStr">
-        <is>
-          <t>2.59x</t>
-        </is>
-      </c>
-      <c r="AG18" t="inlineStr">
-        <is>
-          <t>2.59x</t>
-        </is>
-      </c>
-      <c r="AH18" t="inlineStr">
-        <is>
-          <t>3.25x</t>
-        </is>
-      </c>
-      <c r="AI18" t="inlineStr">
-        <is>
-          <t>2.83x</t>
-        </is>
-      </c>
-      <c r="AJ18" t="inlineStr">
-        <is>
-          <t>2.58x</t>
-        </is>
-      </c>
       <c r="AK18" t="inlineStr">
         <is>
           <t>2.32x</t>
@@ -9725,7 +9717,7 @@
       </c>
       <c r="AU18" t="inlineStr">
         <is>
-          <t>1.41x</t>
+          <t>1.26x</t>
         </is>
       </c>
     </row>
@@ -9743,149 +9735,149 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>3.88x</t>
+          <t>3.86x</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
+          <t>4.43x</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>3.76x</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>3.68x</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>3.23x</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>3.93x</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>3.35x</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>4.67x</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>5.32x</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>4.32x</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>4.00x</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>3.65x</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>3.92x</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>6.45x</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>7.66x</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>6.92x</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>6.54x</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>6.11x</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>6.35x</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>5.69x</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>5.80x</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>6.85x</t>
+        </is>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>5.60x</t>
+        </is>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>6.14x</t>
+        </is>
+      </c>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>4.74x</t>
+        </is>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>5.11x</t>
+        </is>
+      </c>
+      <c r="AH19" t="inlineStr">
+        <is>
+          <t>5.85x</t>
+        </is>
+      </c>
+      <c r="AI19" t="inlineStr">
+        <is>
+          <t>5.08x</t>
+        </is>
+      </c>
+      <c r="AJ19" t="inlineStr">
+        <is>
           <t>4.36x</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>3.76x</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>3.68x</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>3.23x</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>3.95x</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>3.35x</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>4.67x</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>5.32x</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>4.32x</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>4.00x</t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>3.65x</t>
-        </is>
-      </c>
-      <c r="T19" t="inlineStr">
-        <is>
-          <t>3.92x</t>
-        </is>
-      </c>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>6.45x</t>
-        </is>
-      </c>
-      <c r="V19" t="inlineStr">
-        <is>
-          <t>7.66x</t>
-        </is>
-      </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t>6.94x</t>
-        </is>
-      </c>
-      <c r="X19" t="inlineStr">
-        <is>
-          <t>6.54x</t>
-        </is>
-      </c>
-      <c r="Y19" t="inlineStr">
-        <is>
-          <t>6.11x</t>
-        </is>
-      </c>
-      <c r="Z19" t="inlineStr">
-        <is>
-          <t>6.39x</t>
-        </is>
-      </c>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t>5.69x</t>
-        </is>
-      </c>
-      <c r="AB19" t="inlineStr">
-        <is>
-          <t>5.80x</t>
-        </is>
-      </c>
-      <c r="AC19" t="inlineStr">
-        <is>
-          <t>6.85x</t>
-        </is>
-      </c>
-      <c r="AD19" t="inlineStr">
-        <is>
-          <t>5.56x</t>
-        </is>
-      </c>
-      <c r="AE19" t="inlineStr">
-        <is>
-          <t>6.19x</t>
-        </is>
-      </c>
-      <c r="AF19" t="inlineStr">
-        <is>
-          <t>4.74x</t>
-        </is>
-      </c>
-      <c r="AG19" t="inlineStr">
-        <is>
-          <t>5.11x</t>
-        </is>
-      </c>
-      <c r="AH19" t="inlineStr">
-        <is>
-          <t>5.85x</t>
-        </is>
-      </c>
-      <c r="AI19" t="inlineStr">
-        <is>
-          <t>5.08x</t>
-        </is>
-      </c>
-      <c r="AJ19" t="inlineStr">
-        <is>
-          <t>4.36x</t>
-        </is>
-      </c>
       <c r="AK19" t="inlineStr">
         <is>
           <t>3.75x</t>
@@ -9938,7 +9930,7 @@
       </c>
       <c r="AU19" t="inlineStr">
         <is>
-          <t>2.02x</t>
+          <t>1.81x</t>
         </is>
       </c>
     </row>
@@ -9954,9 +9946,21 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>20.83x</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>20.37x</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>16.97x</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr">
         <is>
           <t>13.49x</t>
@@ -9964,32 +9968,32 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>12.60x</t>
+          <t>12.48x</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>15.60x</t>
+          <t>17.94x</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>14.13x</t>
+          <t>16.46x</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>18.08x</t>
+          <t>13.44x</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>21.00x</t>
+          <t>15.61x</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>20.05x</t>
+          <t>14.91x</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -10014,13 +10018,29 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>21.26x</t>
-        </is>
-      </c>
-      <c r="W20" t="inlineStr"/>
-      <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="inlineStr"/>
-      <c r="Z20" t="inlineStr"/>
+          <t>20.84x</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>19.82x</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>18.78x</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>18.41x</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>31.61x</t>
+        </is>
+      </c>
       <c r="AA20" t="inlineStr">
         <is>
           <t>28.72x</t>
@@ -10038,7 +10058,7 @@
       </c>
       <c r="AD20" t="inlineStr">
         <is>
-          <t>19.30x</t>
+          <t>19.03x</t>
         </is>
       </c>
       <c r="AE20" t="inlineStr">
@@ -10103,16 +10123,16 @@
         <v>-16.59</v>
       </c>
       <c r="AR20" s="2" t="n">
-        <v>-19.41</v>
+        <v>-24.37</v>
       </c>
       <c r="AS20" s="2" t="n">
         <v>-59.61</v>
       </c>
       <c r="AT20" s="2" t="n">
-        <v>-18.45</v>
+        <v>-19.85</v>
       </c>
       <c r="AU20" s="2" t="n">
-        <v>-15.16</v>
+        <v>-11.81</v>
       </c>
     </row>
     <row r="21">
@@ -10127,9 +10147,21 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>22.51x</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>21.74x</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>18.14x</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr">
         <is>
           <t>14.43x</t>
@@ -10137,32 +10169,32 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>13.57x</t>
+          <t>13.43x</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>16.35x</t>
+          <t>18.92x</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>15.19x</t>
+          <t>17.90x</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>18.06x</t>
+          <t>13.46x</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>20.86x</t>
+          <t>15.55x</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>20.08x</t>
+          <t>14.96x</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -10187,13 +10219,29 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>21.26x</t>
-        </is>
-      </c>
-      <c r="W21" t="inlineStr"/>
-      <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="inlineStr"/>
-      <c r="Z21" t="inlineStr"/>
+          <t>20.82x</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>19.84x</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>18.42x</t>
+        </is>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>18.02x</t>
+        </is>
+      </c>
+      <c r="Z21" t="inlineStr">
+        <is>
+          <t>31.10x</t>
+        </is>
+      </c>
       <c r="AA21" t="inlineStr">
         <is>
           <t>27.73x</t>
@@ -10211,12 +10259,12 @@
       </c>
       <c r="AD21" t="inlineStr">
         <is>
-          <t>18.47x</t>
+          <t>17.76x</t>
         </is>
       </c>
       <c r="AE21" t="inlineStr">
         <is>
-          <t>18.62x</t>
+          <t>18.39x</t>
         </is>
       </c>
       <c r="AF21" t="inlineStr">
@@ -10276,16 +10324,16 @@
         <v>-13.69</v>
       </c>
       <c r="AR21" s="2" t="n">
-        <v>-15.71</v>
+        <v>-19.85</v>
       </c>
       <c r="AS21" s="2" t="n">
         <v>-47.34</v>
       </c>
       <c r="AT21" s="2" t="n">
-        <v>-15.31</v>
+        <v>-17.24</v>
       </c>
       <c r="AU21" s="2" t="n">
-        <v>-12.17</v>
+        <v>-9.039999999999999</v>
       </c>
     </row>
     <row r="22">
@@ -10471,7 +10519,7 @@
         <v>0.017</v>
       </c>
       <c r="AU23" s="3" t="n">
-        <v>0.021</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="24">
@@ -10623,7 +10671,7 @@
         <v>44.17</v>
       </c>
       <c r="AU25" s="2" t="n">
-        <v>35.11</v>
+        <v>31.42</v>
       </c>
     </row>
     <row r="26">
@@ -10768,7 +10816,7 @@
         <v>216456.05</v>
       </c>
       <c r="AU26" s="1" t="n">
-        <v>177888.79</v>
+        <v>168201.93</v>
       </c>
     </row>
     <row r="27">
@@ -10913,7 +10961,7 @@
         <v>188026.05</v>
       </c>
       <c r="AU27" s="1" t="n">
-        <v>149458.79</v>
+        <v>133750.93</v>
       </c>
     </row>
     <row r="28">
@@ -10989,7 +11037,7 @@
         <v>57498.28</v>
       </c>
       <c r="AU29" s="1" t="n">
-        <v>59478.33</v>
+        <v>57781.14</v>
       </c>
     </row>
     <row r="30">
@@ -11058,7 +11106,7 @@
         <v>16232.43</v>
       </c>
       <c r="AU30" s="1" t="n">
-        <v>18403.36</v>
+        <v>16211.31</v>
       </c>
     </row>
     <row r="31">
@@ -11112,7 +11160,7 @@
         <v>6961.16</v>
       </c>
       <c r="AP31" s="1" t="n">
-        <v>2315</v>
+        <v>2412.95</v>
       </c>
       <c r="AQ31" s="1" t="n">
         <v>3464.47</v>
@@ -11127,7 +11175,7 @@
         <v>6254.48</v>
       </c>
       <c r="AU31" s="1" t="n">
-        <v>7719.52</v>
+        <v>5954.61</v>
       </c>
     </row>
     <row r="32">
@@ -11196,7 +11244,7 @@
         <v>1.37</v>
       </c>
       <c r="AU32" s="2" t="n">
-        <v>1.62</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="33">
@@ -11334,7 +11382,7 @@
         <v>-5508.33</v>
       </c>
       <c r="AU34" s="1" t="n">
-        <v>-5943.34</v>
+        <v>-7226.73</v>
       </c>
     </row>
     <row r="35">
@@ -11474,7 +11522,7 @@
         <v>54228</v>
       </c>
       <c r="AU36" s="1" t="n">
-        <v>54228</v>
+        <v>55237</v>
       </c>
     </row>
     <row r="37">
@@ -11543,10 +11591,10 @@
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
       <c r="H38" s="1" t="n">
-        <v>21856</v>
+        <v>22019</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>23263</v>
+        <v>23128</v>
       </c>
       <c r="J38" s="1" t="n">
         <v>24142</v>
@@ -11555,16 +11603,16 @@
         <v>24356</v>
       </c>
       <c r="L38" s="1" t="n">
-        <v>23596</v>
+        <v>23504</v>
       </c>
       <c r="M38" s="1" t="n">
-        <v>23327</v>
+        <v>23319</v>
       </c>
       <c r="N38" s="1" t="n">
         <v>23067</v>
       </c>
       <c r="O38" s="1" t="n">
-        <v>23219.75</v>
+        <v>23057</v>
       </c>
       <c r="P38" s="1" t="n">
         <v>22630</v>
@@ -11588,7 +11636,7 @@
         <v>26504</v>
       </c>
       <c r="W38" s="1" t="n">
-        <v>27348.25</v>
+        <v>27512</v>
       </c>
       <c r="X38" s="1" t="n">
         <v>29046</v>
@@ -11597,7 +11645,7 @@
         <v>31070</v>
       </c>
       <c r="Z38" s="1" t="n">
-        <v>32033.33</v>
+        <v>32329</v>
       </c>
       <c r="AA38" s="1" t="n">
         <v>32462</v>
@@ -11651,7 +11699,7 @@
         <v>9855</v>
       </c>
       <c r="AR38" s="1" t="n">
-        <v>8780</v>
+        <v>8870</v>
       </c>
       <c r="AS38" s="1" t="n">
         <v>8294</v>
@@ -11660,7 +11708,7 @@
         <v>9633</v>
       </c>
       <c r="AU38" s="1" t="n">
-        <v>9633</v>
+        <v>10501</v>
       </c>
     </row>
     <row r="39">
@@ -11793,7 +11841,7 @@
         <v>31</v>
       </c>
       <c r="AU39" s="2" t="n">
-        <v>31</v>
+        <v>714</v>
       </c>
     </row>
     <row r="40">
@@ -11926,7 +11974,7 @@
         <v>0.4</v>
       </c>
       <c r="AU40" s="2" t="n">
-        <v>0.4</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="41">
@@ -11942,10 +11990,10 @@
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
       <c r="H41" s="2" t="n">
-        <v>11.89</v>
+        <v>11.97</v>
       </c>
       <c r="I41" s="2" t="n">
-        <v>11.68</v>
+        <v>11.54</v>
       </c>
       <c r="J41" s="2" t="n">
         <v>11.71</v>
@@ -11954,16 +12002,16 @@
         <v>11.58</v>
       </c>
       <c r="L41" s="2" t="n">
-        <v>12.14</v>
+        <v>12.12</v>
       </c>
       <c r="M41" s="2" t="n">
-        <v>12.03</v>
+        <v>12.07</v>
       </c>
       <c r="N41" s="2" t="n">
         <v>12.93</v>
       </c>
       <c r="O41" s="2" t="n">
-        <v>12.96</v>
+        <v>12.97</v>
       </c>
       <c r="P41" s="2" t="n">
         <v>12.98</v>
@@ -11987,7 +12035,7 @@
         <v>14.73</v>
       </c>
       <c r="W41" s="2" t="n">
-        <v>15.01</v>
+        <v>15.06</v>
       </c>
       <c r="X41" s="2" t="n">
         <v>15.07</v>
@@ -11996,7 +12044,7 @@
         <v>15.63</v>
       </c>
       <c r="Z41" s="2" t="n">
-        <v>16.39</v>
+        <v>16.51</v>
       </c>
       <c r="AA41" s="2" t="n">
         <v>16.45</v>
@@ -12008,10 +12056,10 @@
         <v>16.91</v>
       </c>
       <c r="AD41" s="2" t="n">
-        <v>18.07</v>
+        <v>17.94</v>
       </c>
       <c r="AE41" s="2" t="n">
-        <v>17.9</v>
+        <v>18.03</v>
       </c>
       <c r="AF41" s="2" t="n">
         <v>19.28</v>
@@ -12059,7 +12107,7 @@
         <v>24.97</v>
       </c>
       <c r="AU41" s="2" t="n">
-        <v>24.97</v>
+        <v>24.89</v>
       </c>
     </row>
     <row r="42">
@@ -12075,10 +12123,10 @@
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
       <c r="H42" s="2" t="n">
-        <v>8.82</v>
+        <v>8.880000000000001</v>
       </c>
       <c r="I42" s="2" t="n">
-        <v>8.619999999999999</v>
+        <v>8.470000000000001</v>
       </c>
       <c r="J42" s="2" t="n">
         <v>8.5</v>
@@ -12087,16 +12135,16 @@
         <v>8.42</v>
       </c>
       <c r="L42" s="2" t="n">
-        <v>8.93</v>
+        <v>8.92</v>
       </c>
       <c r="M42" s="2" t="n">
-        <v>8.859999999999999</v>
+        <v>8.890000000000001</v>
       </c>
       <c r="N42" s="2" t="n">
         <v>9.699999999999999</v>
       </c>
       <c r="O42" s="2" t="n">
-        <v>7.01</v>
+        <v>7.02</v>
       </c>
       <c r="P42" s="2" t="n">
         <v>7.1</v>
@@ -12120,7 +12168,7 @@
         <v>6.8</v>
       </c>
       <c r="W42" s="2" t="n">
-        <v>7.16</v>
+        <v>7.18</v>
       </c>
       <c r="X42" s="2" t="n">
         <v>7.23</v>
@@ -12129,7 +12177,7 @@
         <v>7.65</v>
       </c>
       <c r="Z42" s="2" t="n">
-        <v>8.4</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="AA42" s="2" t="n">
         <v>8.42</v>
@@ -12141,10 +12189,10 @@
         <v>8.77</v>
       </c>
       <c r="AD42" s="2" t="n">
-        <v>9.42</v>
+        <v>9.35</v>
       </c>
       <c r="AE42" s="2" t="n">
-        <v>9.289999999999999</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="AF42" s="2" t="n">
         <v>10.53</v>
@@ -12192,7 +12240,7 @@
         <v>17.36</v>
       </c>
       <c r="AU42" s="2" t="n">
-        <v>17.36</v>
+        <v>17.35</v>
       </c>
     </row>
     <row r="43">
@@ -12325,7 +12373,7 @@
         <v>0.74</v>
       </c>
       <c r="AU43" s="2" t="n">
-        <v>0.74</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="44">
@@ -12340,29 +12388,35 @@
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr"/>
+      <c r="H44" s="1" t="n">
+        <v>7659.63</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <v>8474.129999999999</v>
+      </c>
+      <c r="J44" s="1" t="n">
+        <v>8474.129999999999</v>
+      </c>
       <c r="K44" s="1" t="n">
         <v>10317.88</v>
       </c>
       <c r="L44" s="1" t="n">
-        <v>10219.75</v>
+        <v>10317.88</v>
       </c>
       <c r="M44" s="1" t="n">
-        <v>10219.75</v>
+        <v>8888.5</v>
       </c>
       <c r="N44" s="1" t="n">
-        <v>10219.75</v>
+        <v>8772.5</v>
       </c>
       <c r="O44" s="1" t="n">
-        <v>8772.5</v>
+        <v>11800.75</v>
       </c>
       <c r="P44" s="1" t="n">
-        <v>8772.5</v>
+        <v>11800.75</v>
       </c>
       <c r="Q44" s="1" t="n">
-        <v>8772.5</v>
+        <v>11800.75</v>
       </c>
       <c r="R44" s="1" t="n">
         <v>6290.5</v>
@@ -12377,12 +12431,20 @@
         <v>11841</v>
       </c>
       <c r="V44" s="1" t="n">
-        <v>11841</v>
-      </c>
-      <c r="W44" t="inlineStr"/>
-      <c r="X44" t="inlineStr"/>
-      <c r="Y44" t="inlineStr"/>
-      <c r="Z44" t="inlineStr"/>
+        <v>12081.38</v>
+      </c>
+      <c r="W44" s="1" t="n">
+        <v>12081.38</v>
+      </c>
+      <c r="X44" s="1" t="n">
+        <v>12222.13</v>
+      </c>
+      <c r="Y44" s="1" t="n">
+        <v>12222.13</v>
+      </c>
+      <c r="Z44" s="1" t="n">
+        <v>8058.5</v>
+      </c>
       <c r="AA44" s="1" t="n">
         <v>8037.5</v>
       </c>
@@ -12393,7 +12455,7 @@
         <v>11953.75</v>
       </c>
       <c r="AD44" s="1" t="n">
-        <v>12433.5</v>
+        <v>12608.5</v>
       </c>
       <c r="AE44" s="1" t="n">
         <v>13540.75</v>
@@ -12435,16 +12497,16 @@
         <v>-9834.75</v>
       </c>
       <c r="AR44" s="1" t="n">
-        <v>-9056.629999999999</v>
+        <v>-7215.63</v>
       </c>
       <c r="AS44" s="1" t="n">
         <v>-4000.25</v>
       </c>
       <c r="AT44" s="1" t="n">
-        <v>-11734.63</v>
+        <v>-10903.63</v>
       </c>
       <c r="AU44" s="1" t="n">
-        <v>-11734.63</v>
+        <v>-14245.75</v>
       </c>
     </row>
     <row r="45">
@@ -12459,29 +12521,35 @@
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
+      <c r="H45" s="1" t="n">
+        <v>7536.5</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>8352.879999999999</v>
+      </c>
+      <c r="J45" s="1" t="n">
+        <v>8352.879999999999</v>
+      </c>
       <c r="K45" s="1" t="n">
         <v>10194.75</v>
       </c>
       <c r="L45" s="1" t="n">
-        <v>10094.13</v>
+        <v>10194.75</v>
       </c>
       <c r="M45" s="1" t="n">
-        <v>10094.13</v>
+        <v>8723.5</v>
       </c>
       <c r="N45" s="1" t="n">
-        <v>10094.13</v>
+        <v>8561.879999999999</v>
       </c>
       <c r="O45" s="1" t="n">
-        <v>8561.879999999999</v>
+        <v>11486.38</v>
       </c>
       <c r="P45" s="1" t="n">
-        <v>8561.879999999999</v>
+        <v>11486.38</v>
       </c>
       <c r="Q45" s="1" t="n">
-        <v>8561.879999999999</v>
+        <v>11486.38</v>
       </c>
       <c r="R45" s="1" t="n">
         <v>5832.38</v>
@@ -12496,12 +12564,20 @@
         <v>11434.13</v>
       </c>
       <c r="V45" s="1" t="n">
-        <v>11434.13</v>
-      </c>
-      <c r="W45" t="inlineStr"/>
-      <c r="X45" t="inlineStr"/>
-      <c r="Y45" t="inlineStr"/>
-      <c r="Z45" t="inlineStr"/>
+        <v>11677.63</v>
+      </c>
+      <c r="W45" s="1" t="n">
+        <v>11677.63</v>
+      </c>
+      <c r="X45" s="1" t="n">
+        <v>11839.63</v>
+      </c>
+      <c r="Y45" s="1" t="n">
+        <v>11839.63</v>
+      </c>
+      <c r="Z45" s="1" t="n">
+        <v>7766</v>
+      </c>
       <c r="AA45" s="1" t="n">
         <v>7728.75</v>
       </c>
@@ -12512,10 +12588,10 @@
         <v>11555</v>
       </c>
       <c r="AD45" s="1" t="n">
-        <v>12127.88</v>
+        <v>12608.5</v>
       </c>
       <c r="AE45" s="1" t="n">
-        <v>13077.63</v>
+        <v>13237</v>
       </c>
       <c r="AF45" s="1" t="n">
         <v>16817.75</v>
@@ -12554,16 +12630,16 @@
         <v>-10187.88</v>
       </c>
       <c r="AR45" s="1" t="n">
-        <v>-9475.379999999999</v>
+        <v>-7500.63</v>
       </c>
       <c r="AS45" s="1" t="n">
         <v>-4475.25</v>
       </c>
       <c r="AT45" s="1" t="n">
-        <v>-12283.38</v>
+        <v>-10903.63</v>
       </c>
       <c r="AU45" s="1" t="n">
-        <v>-12283.38</v>
+        <v>-14794.5</v>
       </c>
     </row>
     <row r="46">
@@ -12746,13 +12822,13 @@
         <v>54228</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>57459.09</v>
+        <v>55880.01</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>63823.53</v>
+        <v>62732.08</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>69939.22</v>
+        <v>68999.77</v>
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
@@ -12789,13 +12865,13 @@
         <v>-14</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>0.111</v>
+        <v>0.123</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>0.096</v>
+        <v>0.1</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
@@ -12831,13 +12907,13 @@
         <v>12514</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>16392.26</v>
+        <v>14806.66</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>21851.92</v>
+        <v>20489.12</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>27432.03</v>
+        <v>25881.17</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
@@ -12874,13 +12950,13 @@
         <v>-34.3</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>0.31</v>
+        <v>0.183</v>
       </c>
       <c r="K6" s="3" t="n">
-        <v>0.333</v>
+        <v>0.384</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>0.255</v>
+        <v>0.263</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
@@ -12916,13 +12992,13 @@
         <v>0.231</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>0.285</v>
+        <v>0.265</v>
       </c>
       <c r="K7" s="3" t="n">
-        <v>0.342</v>
+        <v>0.327</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>0.392</v>
+        <v>0.375</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
@@ -12959,13 +13035,13 @@
         <v>4667</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>6271.55</v>
+        <v>5085.22</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>12746.15</v>
+        <v>9144.84</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>18491.94</v>
+        <v>12850.38</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
@@ -13002,13 +13078,13 @@
         <v>-41.1</v>
       </c>
       <c r="J9" s="3" t="n">
-        <v>0.344</v>
+        <v>0.09</v>
       </c>
       <c r="K9" s="3" t="n">
-        <v>1.032</v>
+        <v>0.7979999999999999</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>0.451</v>
+        <v>0.405</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
@@ -13044,13 +13120,13 @@
         <v>0.08599999999999999</v>
       </c>
       <c r="J10" s="3" t="n">
-        <v>0.109</v>
+        <v>0.091</v>
       </c>
       <c r="K10" s="3" t="n">
-        <v>0.2</v>
+        <v>0.146</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>0.264</v>
+        <v>0.186</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
@@ -13087,13 +13163,13 @@
         <v>5143</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>6597.38</v>
+        <v>5388.79</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>11144.33</v>
+        <v>9730.83</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>16354.91</v>
+        <v>13462.76</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
@@ -13130,13 +13206,13 @@
         <v>-35</v>
       </c>
       <c r="J12" s="3" t="n">
-        <v>0.283</v>
+        <v>0.048</v>
       </c>
       <c r="K12" s="3" t="n">
-        <v>0.6890000000000001</v>
+        <v>0.8059999999999999</v>
       </c>
       <c r="L12" s="3" t="n">
-        <v>0.468</v>
+        <v>0.384</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
@@ -13172,13 +13248,13 @@
         <v>0.095</v>
       </c>
       <c r="J13" s="3" t="n">
-        <v>0.115</v>
+        <v>0.096</v>
       </c>
       <c r="K13" s="3" t="n">
-        <v>0.175</v>
+        <v>0.155</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>0.234</v>
+        <v>0.195</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
@@ -13215,13 +13291,13 @@
         <v>4423</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>5750.26</v>
+        <v>4612.2</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>9746.41</v>
+        <v>8460.25</v>
       </c>
       <c r="L14" s="1" t="n">
-        <v>13511.66</v>
+        <v>11709.86</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
@@ -13258,13 +13334,13 @@
         <v>-41.8</v>
       </c>
       <c r="J15" s="3" t="n">
-        <v>0.3</v>
+        <v>0.043</v>
       </c>
       <c r="K15" s="3" t="n">
-        <v>0.695</v>
+        <v>0.8340000000000001</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>0.386</v>
+        <v>0.384</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
@@ -13300,13 +13376,13 @@
         <v>0.08199999999999999</v>
       </c>
       <c r="J16" s="3" t="n">
-        <v>0.1</v>
+        <v>0.083</v>
       </c>
       <c r="K16" s="3" t="n">
-        <v>0.153</v>
+        <v>0.135</v>
       </c>
       <c r="L16" s="3" t="n">
-        <v>0.193</v>
+        <v>0.17</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
@@ -13343,13 +13419,13 @@
         <v>1.05</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>1.35</v>
+        <v>1.1</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>2.29</v>
+        <v>1.99</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>2.9</v>
+        <v>2.63</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
@@ -13386,13 +13462,13 @@
         <v>-42.9</v>
       </c>
       <c r="J18" s="3" t="n">
-        <v>0.289</v>
+        <v>0.044</v>
       </c>
       <c r="K18" s="3" t="n">
-        <v>0.6920000000000001</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="L18" s="3" t="n">
-        <v>0.268</v>
+        <v>0.322</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
@@ -13428,13 +13504,13 @@
         <v>0.4</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>0.46</v>
+        <v>0.11</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>1.28</v>
+        <v>1.05</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>2.04</v>
+        <v>1.71</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
@@ -13470,14 +13546,14 @@
       <c r="I20" s="2" t="n">
         <v>-79.40000000000001</v>
       </c>
-      <c r="J20" s="3" t="n">
-        <v>0.158</v>
+      <c r="J20" s="2" t="n">
+        <v>-71.59999999999999</v>
       </c>
       <c r="K20" s="3" t="n">
-        <v>1.753</v>
+        <v>8.216000000000001</v>
       </c>
       <c r="L20" s="3" t="n">
-        <v>0.603</v>
+        <v>0.632</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
@@ -13513,13 +13589,13 @@
         <v>-14279</v>
       </c>
       <c r="J21" s="1" t="n">
-        <v>-6504.88</v>
+        <v>-12578.06</v>
       </c>
       <c r="K21" s="1" t="n">
-        <v>-2724.69</v>
+        <v>-6182.14</v>
       </c>
       <c r="L21" s="1" t="n">
-        <v>-1418.05</v>
+        <v>-2865.13</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
@@ -13556,13 +13632,13 @@
         <v>0.517</v>
       </c>
       <c r="J22" s="3" t="n">
-        <v>0.544</v>
+        <v>0.119</v>
       </c>
       <c r="K22" s="3" t="n">
-        <v>0.581</v>
+        <v>0.508</v>
       </c>
       <c r="L22" s="3" t="n">
-        <v>0.48</v>
+        <v>0.537</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
@@ -13598,13 +13674,13 @@
         <v>-26.3</v>
       </c>
       <c r="J23" s="2" t="n">
-        <v>-11.3</v>
+        <v>-22.5</v>
       </c>
       <c r="K23" s="2" t="n">
-        <v>-4.3</v>
+        <v>-9.9</v>
       </c>
       <c r="L23" s="2" t="n">
-        <v>-2</v>
+        <v>-4.2</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
@@ -13642,10 +13718,10 @@
         <v>0.5</v>
       </c>
       <c r="K24" s="2" t="n">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="L24" s="2" t="n">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
@@ -13681,10 +13757,10 @@
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" s="3" t="n">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="L25" s="3" t="n">
-        <v>0.05599999999999999</v>
+        <v>0.035</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
@@ -13727,13 +13803,13 @@
         <v>43.6</v>
       </c>
       <c r="J27" s="2" t="n">
-        <v>45.89</v>
+        <v>45.3</v>
       </c>
       <c r="K27" s="2" t="n">
-        <v>48.52</v>
+        <v>47.79</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>51.5</v>
+        <v>49.12</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
@@ -13770,10 +13846,10 @@
         <v>629</v>
       </c>
       <c r="J28" s="2" t="n">
-        <v>-225</v>
+        <v>-5</v>
       </c>
       <c r="K28" s="2" t="n">
-        <v>-185</v>
+        <v>-234</v>
       </c>
       <c r="L28" s="2" t="n">
         <v>-175</v>
@@ -13813,13 +13889,13 @@
         <v>7847</v>
       </c>
       <c r="J29" s="1" t="n">
-        <v>10171.52</v>
+        <v>9928.889999999999</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>11632.81</v>
+        <v>11444.2</v>
       </c>
       <c r="L29" s="1" t="n">
-        <v>12789.4</v>
+        <v>12710.67</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
@@ -13856,13 +13932,13 @@
         <v>-29.5</v>
       </c>
       <c r="J30" s="3" t="n">
-        <v>0.296</v>
+        <v>0.265</v>
       </c>
       <c r="K30" s="3" t="n">
-        <v>0.144</v>
+        <v>0.153</v>
       </c>
       <c r="L30" s="3" t="n">
-        <v>0.099</v>
+        <v>0.111</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
@@ -13898,10 +13974,10 @@
         <v>13</v>
       </c>
       <c r="J31" s="2" t="n">
-        <v>12.92</v>
+        <v>13</v>
       </c>
       <c r="K31" s="2" t="n">
-        <v>13.1</v>
+        <v>13.15</v>
       </c>
       <c r="L31" s="2" t="n">
         <v>13</v>
@@ -13982,13 +14058,13 @@
         <v>762</v>
       </c>
       <c r="J34" s="1" t="n">
-        <v>2973.88</v>
+        <v>1262.17</v>
       </c>
       <c r="K34" s="1" t="n">
-        <v>6398.78</v>
+        <v>4873.87</v>
       </c>
       <c r="L34" s="1" t="n">
-        <v>10068.44</v>
+        <v>8209.530000000001</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
@@ -14025,13 +14101,13 @@
         <v>-90.2</v>
       </c>
       <c r="J35" s="3" t="n">
-        <v>2.903</v>
+        <v>0.6559999999999999</v>
       </c>
       <c r="K35" s="3" t="n">
-        <v>1.152</v>
+        <v>2.862</v>
       </c>
       <c r="L35" s="3" t="n">
-        <v>0.573</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
@@ -14128,14 +14204,14 @@
       <c r="I39" s="1" t="n">
         <v>1689</v>
       </c>
-      <c r="J39" s="1" t="n">
-        <v>2278.56</v>
+      <c r="J39" s="2" t="n">
+        <v>409.95</v>
       </c>
       <c r="K39" s="1" t="n">
-        <v>5959.22</v>
+        <v>4319.78</v>
       </c>
       <c r="L39" s="1" t="n">
-        <v>8618.110000000001</v>
+        <v>7174.28</v>
       </c>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
@@ -14171,14 +14247,14 @@
       <c r="I40" s="2" t="n">
         <v>-78.90000000000001</v>
       </c>
-      <c r="J40" s="3" t="n">
-        <v>0.349</v>
+      <c r="J40" s="2" t="n">
+        <v>-75.7</v>
       </c>
       <c r="K40" s="3" t="n">
-        <v>1.615</v>
+        <v>9.537000000000001</v>
       </c>
       <c r="L40" s="3" t="n">
-        <v>0.446</v>
+        <v>0.6609999999999999</v>
       </c>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr"/>
@@ -14210,13 +14286,13 @@
         <v>2.91</v>
       </c>
       <c r="J41" s="2" t="n">
-        <v>4.43</v>
+        <v>3.75</v>
       </c>
       <c r="K41" s="2" t="n">
-        <v>6.16</v>
+        <v>5.35</v>
       </c>
       <c r="L41" s="2" t="n">
-        <v>7.04</v>
+        <v>6.34</v>
       </c>
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr"/>
@@ -14247,13 +14323,13 @@
         <v>-35.8</v>
       </c>
       <c r="J42" s="3" t="n">
-        <v>0.521</v>
+        <v>0.286</v>
       </c>
       <c r="K42" s="3" t="n">
-        <v>0.391</v>
+        <v>0.428</v>
       </c>
       <c r="L42" s="3" t="n">
-        <v>0.143</v>
+        <v>0.186</v>
       </c>
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
@@ -14296,13 +14372,13 @@
         <v>11471</v>
       </c>
       <c r="J44" s="1" t="n">
-        <v>16658.17</v>
+        <v>12740.69</v>
       </c>
       <c r="K44" s="1" t="n">
-        <v>21569.28</v>
+        <v>19744.81</v>
       </c>
       <c r="L44" s="1" t="n">
-        <v>26535.49</v>
+        <v>25414.45</v>
       </c>
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr"/>
@@ -14339,13 +14415,13 @@
         <v>-25.7</v>
       </c>
       <c r="J45" s="3" t="n">
-        <v>0.452</v>
+        <v>0.111</v>
       </c>
       <c r="K45" s="3" t="n">
-        <v>0.295</v>
+        <v>0.55</v>
       </c>
       <c r="L45" s="3" t="n">
-        <v>0.23</v>
+        <v>0.287</v>
       </c>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr"/>
@@ -14381,13 +14457,13 @@
         <v>-25750</v>
       </c>
       <c r="J46" s="1" t="n">
-        <v>-21994.54</v>
+        <v>-21563.05</v>
       </c>
       <c r="K46" s="1" t="n">
-        <v>-22344.87</v>
+        <v>-22500.68</v>
       </c>
       <c r="L46" s="1" t="n">
-        <v>-23102.43</v>
+        <v>-23413.32</v>
       </c>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
@@ -14424,13 +14500,13 @@
         <v>0.036</v>
       </c>
       <c r="J47" s="3" t="n">
-        <v>0.146</v>
+        <v>0.163</v>
       </c>
       <c r="K47" s="3" t="n">
-        <v>0.016</v>
+        <v>0.043</v>
       </c>
       <c r="L47" s="3" t="n">
-        <v>0.034</v>
+        <v>0.04099999999999999</v>
       </c>
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="inlineStr"/>
@@ -14466,13 +14542,13 @@
         <v>2.72</v>
       </c>
       <c r="J48" s="2" t="n">
-        <v>3.49</v>
+        <v>2.63</v>
       </c>
       <c r="K48" s="2" t="n">
-        <v>4.93</v>
+        <v>4.35</v>
       </c>
       <c r="L48" s="2" t="n">
-        <v>6.25</v>
+        <v>5.25</v>
       </c>
       <c r="M48" t="inlineStr"/>
       <c r="N48" t="inlineStr"/>
@@ -14508,14 +14584,14 @@
       <c r="I49" s="2" t="n">
         <v>-27.2</v>
       </c>
-      <c r="J49" s="3" t="n">
-        <v>0.282</v>
+      <c r="J49" s="2" t="n">
+        <v>-3.5</v>
       </c>
       <c r="K49" s="3" t="n">
-        <v>0.411</v>
+        <v>0.655</v>
       </c>
       <c r="L49" s="3" t="n">
-        <v>0.269</v>
+        <v>0.208</v>
       </c>
       <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr"/>
@@ -14558,13 +14634,13 @@
         <v>24232</v>
       </c>
       <c r="J51" s="1" t="n">
-        <v>34747.06</v>
+        <v>37010.91</v>
       </c>
       <c r="K51" s="1" t="n">
-        <v>34836.78</v>
+        <v>37716.43</v>
       </c>
       <c r="L51" s="1" t="n">
-        <v>31713.5</v>
+        <v>36568.15</v>
       </c>
       <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr"/>
@@ -14618,17 +14694,17 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>2.12x</t>
+          <t>2.50x</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>1.59x</t>
+          <t>1.84x</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>1.16x</t>
+          <t>1.41x</t>
         </is>
       </c>
       <c r="M52" t="inlineStr"/>
@@ -14666,13 +14742,13 @@
         <v>25.07</v>
       </c>
       <c r="J53" s="2" t="n">
-        <v>25.68</v>
+        <v>25.59</v>
       </c>
       <c r="K53" s="2" t="n">
-        <v>27.16</v>
+        <v>27.05</v>
       </c>
       <c r="L53" s="2" t="n">
-        <v>30.32</v>
+        <v>29.48</v>
       </c>
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr"/>
@@ -14709,13 +14785,13 @@
         <v>0.023</v>
       </c>
       <c r="J54" s="3" t="n">
-        <v>0.024</v>
+        <v>0.021</v>
       </c>
       <c r="K54" s="3" t="n">
-        <v>0.058</v>
+        <v>0.057</v>
       </c>
       <c r="L54" s="3" t="n">
-        <v>0.117</v>
+        <v>0.09</v>
       </c>
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr"/>
@@ -14751,13 +14827,13 @@
         <v>4.27</v>
       </c>
       <c r="J55" s="2" t="n">
-        <v>5.9</v>
+        <v>4.32</v>
       </c>
       <c r="K55" s="2" t="n">
-        <v>8.9</v>
+        <v>7.59</v>
       </c>
       <c r="L55" s="2" t="n">
-        <v>8.390000000000001</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="inlineStr"/>
@@ -14794,13 +14870,13 @@
         <v>2.37</v>
       </c>
       <c r="J56" s="2" t="n">
-        <v>3.06</v>
+        <v>2.17</v>
       </c>
       <c r="K56" s="2" t="n">
-        <v>4.42</v>
+        <v>3.36</v>
       </c>
       <c r="L56" s="2" t="n">
-        <v>5.41</v>
+        <v>4.67</v>
       </c>
       <c r="M56" t="inlineStr"/>
       <c r="N56" t="inlineStr"/>

</xml_diff>